<commit_message>
Adding the target column to the data set. Preprocessing script approval. Change Handle_Nulls.xlsx
</commit_message>
<xml_diff>
--- a/Handle_Nulls/Handle_null.xlsx
+++ b/Handle_Nulls/Handle_null.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97252\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97252\Desktop\שיעורי בית\שנה ג\סדנה\Git\CAD-Risk-Factors-\Handle_Nulls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AC46D7-3CB8-4554-AECF-7234495E6BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFC94C7-E5BF-4DA3-9324-8215508ABAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Field ID</t>
   </si>
@@ -209,13 +209,16 @@
   </si>
   <si>
     <t>30080-0.0</t>
+  </si>
+  <si>
+    <t>131306-0.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +241,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -281,13 +291,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -507,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1166,7 +1180,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="4">
+        <v>0</v>
+      </c>
+    </row>
     <row r="63" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>